<commit_message>
Append notify setting on publicform
</commit_message>
<xml_diff>
--- a/system_template/data/ja/mail_template.xlsx
+++ b/system_template/data/ja/mail_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h-sat\Dropbox\3_Develop\TFS_Exc\ExmentProject2\vendor\exceedone\exment\system_template\data\ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E666BD-4F21-43AE-93E8-B175ACBE583B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0201BC-4A18-451A-93CC-7BD0DECF8040}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6B672C1-A825-47CF-A377-E0B53872B948}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6B672C1-A825-47CF-A377-E0B53872B948}"/>
   </bookViews>
   <sheets>
     <sheet name="mail_template" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="66">
   <si>
     <t>id</t>
   </si>
@@ -393,6 +393,33 @@
   <si>
     <t>ユーザー${target_user}により、${target_table}のデータが${create_or_update}されました。\n以下の内容をご確認ください。\n\n${create_or_update}ユーザー:${target_user}\n${create_or_update}日時:${target_datetime}\n${create_or_update}データ:${value_url/link=true}\n${free_space}</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>publicform_admin_error</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>公開フォーム 管理者エラー通知</t>
+    <rPh sb="0" eb="2">
+      <t>コウカイ</t>
+    </rPh>
+    <rPh sb="7" eb="10">
+      <t>カンリシャ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[${system:site_name}]公開フォーム ${publicform:public_form_view_name} でエラーが発生しました</t>
+    <rPh sb="21" eb="23">
+      <t>コウカイ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>ハッセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>${user:user_name}様\n\n公開フォーム ${publicform:public_form_view_name} の入力中に、エラーが発生しました。\n入力された内容と、エラー内容をご確認ください。\n\n■入力内容\n${form:values}\n\n■エラー概要\n${error:message}\n\n■エラー詳細\n${error:stacktrace}\n\n</t>
   </si>
 </sst>
 </file>
@@ -759,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C02B19E-36B6-49DD-989B-C96CC8D7F9C4}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1029,6 +1056,23 @@
         <v>59</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>